<commit_message>
Finished-Fixing method/location determination to match up with analysis section
</commit_message>
<xml_diff>
--- a/Data/1day/windata10m.xlsx
+++ b/Data/1day/windata10m.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaronmao/Documents/Programming/APEnviro-LTP/Data/1day/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{A95D32D5-DA7C-CD49-B2A5-C08CFFB04365}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFB0DE9B-BEB9-E848-93D8-C004A340C68D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8460" yWindow="6300" windowWidth="27240" windowHeight="16440"/>
+    <workbookView xWindow="11140" yWindow="5940" windowWidth="27240" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="windata10m" sheetId="1" r:id="rId1"/>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -907,16 +907,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P145"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:R145"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -957,7 +960,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>43607</v>
       </c>
@@ -998,8 +1001,12 @@
         <f>0.5*0.0765*0.000133*0.35*30429.57*(G2*2.24)^3</f>
         <v>1.9954503676743871E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="O2">
+        <f>N2*1/6</f>
+        <v>3.3257506127906452E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>43607.006944444445</v>
       </c>
@@ -1040,12 +1047,20 @@
         <f t="shared" ref="N3:N66" si="0">0.5*0.0765*0.000133*0.35*30429.57*(G3*2.24)^3</f>
         <v>2.9918358326367998E-3</v>
       </c>
+      <c r="O3">
+        <f t="shared" ref="O3:O66" si="1">N3*1/6</f>
+        <v>4.9863930543946663E-4</v>
+      </c>
       <c r="P3">
+        <f>SUM(O2:O145)</f>
+        <v>36.78232901909189</v>
+      </c>
+      <c r="R3">
         <f>SUM(N2:N145)/145*24</f>
         <v>36.528657784477481</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>43607.013888888891</v>
       </c>
@@ -1086,8 +1101,12 @@
         <f t="shared" si="0"/>
         <v>8.1052991924273959E-4</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="O4">
+        <f t="shared" si="1"/>
+        <v>1.3508831987378992E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>43607.020833333336</v>
       </c>
@@ -1128,8 +1147,12 @@
         <f t="shared" si="0"/>
         <v>9.5889769499352934E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="O5">
+        <f t="shared" si="1"/>
+        <v>1.5981628249892157E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>43607.027777777781</v>
       </c>
@@ -1170,8 +1193,12 @@
         <f t="shared" si="0"/>
         <v>5.5491764756570007E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="O6">
+        <f t="shared" si="1"/>
+        <v>9.2486274594283345E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>43607.034722222219</v>
       </c>
@@ -1212,8 +1239,12 @@
         <f t="shared" si="0"/>
         <v>2.610929398011454E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="O7">
+        <f t="shared" si="1"/>
+        <v>4.3515489966857567E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>43607.041666666664</v>
       </c>
@@ -1254,8 +1285,12 @@
         <f t="shared" si="0"/>
         <v>2.9918358326367998E-3</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="O8">
+        <f t="shared" si="1"/>
+        <v>4.9863930543946663E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>43607.048611111109</v>
       </c>
@@ -1296,8 +1331,12 @@
         <f t="shared" si="0"/>
         <v>1.3367958517818648E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="O9">
+        <f t="shared" si="1"/>
+        <v>2.2279930863031081E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>43607.055555555555</v>
       </c>
@@ -1338,8 +1377,12 @@
         <f t="shared" si="0"/>
         <v>2.3934686661094398E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="O10">
+        <f t="shared" si="1"/>
+        <v>3.989114443515733E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>43607.0625</v>
       </c>
@@ -1380,8 +1423,12 @@
         <f t="shared" si="0"/>
         <v>1.4852001653201484E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="O11">
+        <f t="shared" si="1"/>
+        <v>2.4753336088669141E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>43607.069444444445</v>
       </c>
@@ -1422,8 +1469,12 @@
         <f t="shared" si="0"/>
         <v>4.1768780736934257E-3</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="O12">
+        <f t="shared" si="1"/>
+        <v>6.9614634561557091E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>43607.076388888891</v>
       </c>
@@ -1464,8 +1515,12 @@
         <f t="shared" si="0"/>
         <v>4.8416831171474439E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="O13">
+        <f t="shared" si="1"/>
+        <v>8.069471861912406E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>43607.083333333336</v>
       </c>
@@ -1506,8 +1561,12 @@
         <f t="shared" si="0"/>
         <v>5.6396074997047407E-3</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="O14">
+        <f t="shared" si="1"/>
+        <v>9.3993458328412349E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>43607.090277777781</v>
       </c>
@@ -1548,8 +1607,12 @@
         <f t="shared" si="0"/>
         <v>3.1178911994912299E-4</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="O15">
+        <f t="shared" si="1"/>
+        <v>5.1964853324853831E-5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>43607.097222222219</v>
       </c>
@@ -1590,8 +1653,12 @@
         <f t="shared" si="0"/>
         <v>1.3367958517818648E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O16">
+        <f t="shared" si="1"/>
+        <v>2.2279930863031081E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>43607.104166666664</v>
       </c>
@@ -1632,8 +1699,12 @@
         <f t="shared" si="0"/>
         <v>5.6396074997047407E-3</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O17">
+        <f t="shared" si="1"/>
+        <v>9.3993458328412349E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>43607.111111111109</v>
       </c>
@@ -1674,8 +1745,12 @@
         <f t="shared" si="0"/>
         <v>1.3367958517818648E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O18">
+        <f t="shared" si="1"/>
+        <v>2.2279930863031081E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>43607.118055555555</v>
       </c>
@@ -1716,8 +1791,12 @@
         <f t="shared" si="0"/>
         <v>9.5150488265723556E-3</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O19">
+        <f t="shared" si="1"/>
+        <v>1.5858414710953927E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>43607.125</v>
       </c>
@@ -1758,8 +1837,12 @@
         <f t="shared" si="0"/>
         <v>5.5491764756570007E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O20">
+        <f t="shared" si="1"/>
+        <v>9.2486274594283345E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>43607.131944444445</v>
       </c>
@@ -1800,8 +1883,12 @@
         <f t="shared" si="0"/>
         <v>1.3367958517818648E-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O21">
+        <f t="shared" si="1"/>
+        <v>2.2279930863031081E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>43607.138888888891</v>
       </c>
@@ -1842,8 +1929,12 @@
         <f t="shared" si="0"/>
         <v>1.1986221187419117E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O22">
+        <f t="shared" si="1"/>
+        <v>1.9977035312365196E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>43607.145833333336</v>
       </c>
@@ -1884,8 +1975,12 @@
         <f t="shared" si="0"/>
         <v>4.5116859997637926E-2</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O23">
+        <f t="shared" si="1"/>
+        <v>7.5194766662729879E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>43607.152777777781</v>
       </c>
@@ -1926,8 +2021,12 @@
         <f t="shared" si="0"/>
         <v>1.9954503676743871E-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O24">
+        <f t="shared" si="1"/>
+        <v>3.3257506127906452E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>43607.159722222219</v>
       </c>
@@ -1968,8 +2067,12 @@
         <f t="shared" si="0"/>
         <v>6.3224378516558169E-2</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O25">
+        <f t="shared" si="1"/>
+        <v>1.0537396419426361E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>43607.166666666664</v>
       </c>
@@ -2010,8 +2113,12 @@
         <f t="shared" si="0"/>
         <v>7.4092543406659769E-3</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O26">
+        <f t="shared" si="1"/>
+        <v>1.2348757234443295E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>43607.173611111109</v>
       </c>
@@ -2052,8 +2159,12 @@
         <f t="shared" si="0"/>
         <v>0.11881601322561187</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O27">
+        <f t="shared" si="1"/>
+        <v>1.9802668870935312E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>43607.180555555555</v>
       </c>
@@ -2094,8 +2205,12 @@
         <f t="shared" si="0"/>
         <v>1.3378919854066854E-3</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O28">
+        <f t="shared" si="1"/>
+        <v>2.229819975677809E-4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>43607.1875</v>
       </c>
@@ -2136,8 +2251,12 @@
         <f t="shared" si="0"/>
         <v>2.0887435184091638E-4</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O29">
+        <f t="shared" si="1"/>
+        <v>3.4812391973486063E-5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>43607.194444444445</v>
       </c>
@@ -2178,8 +2297,12 @@
         <f t="shared" si="0"/>
         <v>7.6120390612578845E-2</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O30">
+        <f t="shared" si="1"/>
+        <v>1.2686731768763141E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>43607.201388888891</v>
       </c>
@@ -2220,8 +2343,12 @@
         <f t="shared" si="0"/>
         <v>0.20887435184091632</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O31">
+        <f t="shared" si="1"/>
+        <v>3.4812391973486054E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>43607.208333333336</v>
       </c>
@@ -2262,8 +2389,12 @@
         <f t="shared" si="0"/>
         <v>0.25690631831745359</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O32">
+        <f t="shared" si="1"/>
+        <v>4.2817719719575598E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>43607.215277777781</v>
       </c>
@@ -2304,8 +2435,12 @@
         <f t="shared" si="0"/>
         <v>0.18315357633448839</v>
       </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O33">
+        <f t="shared" si="1"/>
+        <v>3.0525596055748064E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>43607.222222222219</v>
       </c>
@@ -2346,8 +2481,12 @@
         <f t="shared" si="0"/>
         <v>6.0896312490063083E-7</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O34">
+        <f t="shared" si="1"/>
+        <v>1.0149385415010514E-7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>43607.229166666664</v>
       </c>
@@ -2388,8 +2527,12 @@
         <f t="shared" si="0"/>
         <v>3.8973639993640369E-2</v>
       </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O35">
+        <f t="shared" si="1"/>
+        <v>6.4956066656067278E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>43607.236111111109</v>
       </c>
@@ -2430,8 +2573,12 @@
         <f t="shared" si="0"/>
         <v>7.6120390612578845E-2</v>
       </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O36">
+        <f t="shared" si="1"/>
+        <v>1.2686731768763141E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>43607.243055555555</v>
       </c>
@@ -2472,8 +2619,12 @@
         <f t="shared" si="0"/>
         <v>5.1873914831535334E-2</v>
       </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O37">
+        <f t="shared" si="1"/>
+        <v>8.6456524719225551E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>43607.25</v>
       </c>
@@ -2514,8 +2665,12 @@
         <f t="shared" si="0"/>
         <v>3.8973639993640369E-2</v>
       </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O38">
+        <f t="shared" si="1"/>
+        <v>6.4956066656067278E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>43607.256944444445</v>
       </c>
@@ -2556,8 +2711,12 @@
         <f t="shared" si="0"/>
         <v>8.4183062386263188E-3</v>
       </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O39">
+        <f t="shared" si="1"/>
+        <v>1.4030510397710532E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>43607.263888888891</v>
       </c>
@@ -2598,8 +2757,12 @@
         <f t="shared" si="0"/>
         <v>7.4092543406659769E-3</v>
       </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O40">
+        <f t="shared" si="1"/>
+        <v>1.2348757234443295E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>43607.270833333336</v>
       </c>
@@ -2640,8 +2803,12 @@
         <f t="shared" si="0"/>
         <v>3.8973639993640369E-2</v>
       </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O41">
+        <f t="shared" si="1"/>
+        <v>6.4956066656067278E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>43607.277777777781</v>
       </c>
@@ -2682,8 +2849,12 @@
         <f t="shared" si="0"/>
         <v>1.0703135883253483E-2</v>
       </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O42">
+        <f t="shared" si="1"/>
+        <v>1.7838559805422472E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>43607.284722222219</v>
       </c>
@@ -2724,8 +2895,12 @@
         <f t="shared" si="0"/>
         <v>1.5658591581026118</v>
       </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O43">
+        <f t="shared" si="1"/>
+        <v>0.26097652635043528</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>43607.291666666664</v>
       </c>
@@ -2766,8 +2941,12 @@
         <f t="shared" si="0"/>
         <v>3.8557261456989576</v>
       </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O44">
+        <f t="shared" si="1"/>
+        <v>0.64262102428315959</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>43607.298611111109</v>
       </c>
@@ -2808,8 +2987,12 @@
         <f t="shared" si="0"/>
         <v>5.3234435886663327</v>
       </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O45">
+        <f t="shared" si="1"/>
+        <v>0.88724059811105549</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>43607.305555555555</v>
       </c>
@@ -2850,8 +3033,12 @@
         <f t="shared" si="0"/>
         <v>5.4013464143454932</v>
       </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O46">
+        <f t="shared" si="1"/>
+        <v>0.9002244023909155</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>43607.3125</v>
       </c>
@@ -2892,8 +3079,12 @@
         <f t="shared" si="0"/>
         <v>3.7935382224209802</v>
       </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O47">
+        <f t="shared" si="1"/>
+        <v>0.63225637040349669</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>43607.319444444445</v>
       </c>
@@ -2934,8 +3125,12 @@
         <f t="shared" si="0"/>
         <v>2.8874790398488273</v>
       </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O48">
+        <f t="shared" si="1"/>
+        <v>0.48124650664147123</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>43607.326388888891</v>
       </c>
@@ -2976,8 +3171,12 @@
         <f t="shared" si="0"/>
         <v>2.1810483219922268</v>
       </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O49">
+        <f t="shared" si="1"/>
+        <v>0.36350805366537114</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>43607.333333333336</v>
       </c>
@@ -3018,8 +3217,12 @@
         <f t="shared" si="0"/>
         <v>2.3566221343110763</v>
       </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O50">
+        <f t="shared" si="1"/>
+        <v>0.39277035571851271</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>43607.340277777781</v>
       </c>
@@ -3060,8 +3263,12 @@
         <f t="shared" si="0"/>
         <v>2.6861022420016867</v>
       </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O51">
+        <f t="shared" si="1"/>
+        <v>0.44768370700028109</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>43607.347222222219</v>
       </c>
@@ -3102,8 +3309,12 @@
         <f t="shared" si="0"/>
         <v>3.8557261456989576</v>
       </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O52">
+        <f t="shared" si="1"/>
+        <v>0.64262102428315959</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>43607.354166666664</v>
       </c>
@@ -3144,8 +3355,12 @@
         <f t="shared" si="0"/>
         <v>6.0521038964343035</v>
       </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O53">
+        <f t="shared" si="1"/>
+        <v>1.0086839827390506</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>43607.361111111109</v>
       </c>
@@ -3186,8 +3401,12 @@
         <f t="shared" si="0"/>
         <v>4.5153854507475639</v>
       </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O54">
+        <f t="shared" si="1"/>
+        <v>0.75256424179126069</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>43607.368055555555</v>
       </c>
@@ -3228,8 +3447,12 @@
         <f t="shared" si="0"/>
         <v>4.3778706158087521</v>
       </c>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O55">
+        <f t="shared" si="1"/>
+        <v>0.72964510263479199</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>43607.375</v>
       </c>
@@ -3270,8 +3493,12 @@
         <f t="shared" si="0"/>
         <v>3.732022594432892</v>
       </c>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O56">
+        <f t="shared" si="1"/>
+        <v>0.62200376573881533</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>43607.381944444445</v>
       </c>
@@ -3312,8 +3539,12 @@
         <f t="shared" si="0"/>
         <v>2.9393486919384881</v>
       </c>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O57">
+        <f t="shared" si="1"/>
+        <v>0.48989144865641471</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>43607.388888888891</v>
       </c>
@@ -3354,8 +3585,12 @@
         <f t="shared" si="0"/>
         <v>3.5514729444204804</v>
       </c>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O58">
+        <f t="shared" si="1"/>
+        <v>0.59191215740341341</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>43607.395833333336</v>
       </c>
@@ -3396,8 +3631,12 @@
         <f t="shared" si="0"/>
         <v>7.3130314683373019</v>
       </c>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O59">
+        <f t="shared" si="1"/>
+        <v>1.218838578056217</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>43607.402777777781</v>
       </c>
@@ -3438,8 +3677,12 @@
         <f t="shared" si="0"/>
         <v>4.5153854507475639</v>
       </c>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O60">
+        <f t="shared" si="1"/>
+        <v>0.75256424179126069</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>43607.409722222219</v>
       </c>
@@ -3480,8 +3723,12 @@
         <f t="shared" si="0"/>
         <v>7.0293685282379617</v>
       </c>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O61">
+        <f t="shared" si="1"/>
+        <v>1.1715614213729937</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>43607.416666666664</v>
       </c>
@@ -3522,8 +3769,12 @@
         <f t="shared" si="0"/>
         <v>4.2431764980644822</v>
       </c>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O62">
+        <f t="shared" si="1"/>
+        <v>0.70719608301074699</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>43607.423611111109</v>
       </c>
@@ -3564,8 +3815,12 @@
         <f t="shared" si="0"/>
         <v>5.4013464143454932</v>
       </c>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O63">
+        <f t="shared" si="1"/>
+        <v>0.9002244023909155</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>43607.430555555555</v>
       </c>
@@ -3606,8 +3861,12 @@
         <f t="shared" si="0"/>
         <v>3.3768424159820993</v>
       </c>
-    </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O64">
+        <f t="shared" si="1"/>
+        <v>0.56280706933034985</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>43607.4375</v>
       </c>
@@ -3648,8 +3907,12 @@
         <f t="shared" si="0"/>
         <v>4.3778706158087521</v>
       </c>
-    </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O65">
+        <f t="shared" si="1"/>
+        <v>0.72964510263479199</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>43607.444444444445</v>
       </c>
@@ -3690,8 +3953,12 @@
         <f t="shared" si="0"/>
         <v>8.9554878351792908</v>
       </c>
-    </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O66">
+        <f t="shared" si="1"/>
+        <v>1.4925813058632151</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>43607.451388888891</v>
       </c>
@@ -3729,11 +3996,15 @@
         <v>32.700000000000003</v>
       </c>
       <c r="N67">
-        <f t="shared" ref="N67:N130" si="1">0.5*0.0765*0.000133*0.35*30429.57*(G67*2.24)^3</f>
+        <f t="shared" ref="N67:N130" si="2">0.5*0.0765*0.000133*0.35*30429.57*(G67*2.24)^3</f>
         <v>6.5730633243030452</v>
       </c>
-    </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O67">
+        <f t="shared" ref="O67:O130" si="3">N67*1/6</f>
+        <v>1.0955105540505075</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>43607.458333333336</v>
       </c>
@@ -3771,11 +4042,15 @@
         <v>31.9</v>
       </c>
       <c r="N68">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.9364705945712481</v>
       </c>
-    </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O68">
+        <f t="shared" si="3"/>
+        <v>1.1560784324285414</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>43607.465277777781</v>
       </c>
@@ -3813,11 +4088,15 @@
         <v>31.1</v>
       </c>
       <c r="N69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.8462757793964819</v>
       </c>
-    </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O69">
+        <f t="shared" si="3"/>
+        <v>1.4743792965660802</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>43607.472222222219</v>
       </c>
@@ -3855,11 +4134,15 @@
         <v>30.7</v>
       </c>
       <c r="N70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.7935382224209802</v>
       </c>
-    </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O70">
+        <f t="shared" si="3"/>
+        <v>0.63225637040349669</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>43607.479166666664</v>
       </c>
@@ -3897,11 +4180,15 @@
         <v>29</v>
       </c>
       <c r="N71">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.3566221343110763</v>
       </c>
-    </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O71">
+        <f t="shared" si="3"/>
+        <v>0.39277035571851271</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>43607.486111111109</v>
       </c>
@@ -3939,11 +4226,15 @@
         <v>28.8</v>
       </c>
       <c r="N72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.92615679258324668</v>
       </c>
-    </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O72">
+        <f t="shared" si="3"/>
+        <v>0.1543594654305411</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>43607.493055555555</v>
       </c>
@@ -3981,11 +4272,15 @@
         <v>27.5</v>
       </c>
       <c r="N73">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.7355384774442455</v>
       </c>
-    </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O73">
+        <f t="shared" si="3"/>
+        <v>0.45592307957404093</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>43607.5</v>
       </c>
@@ -4023,11 +4318,15 @@
         <v>26.6</v>
       </c>
       <c r="N74">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.6003989375838503</v>
       </c>
-    </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O74">
+        <f t="shared" si="3"/>
+        <v>0.26673315626397504</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>43607.506944444445</v>
       </c>
@@ -4065,11 +4364,15 @@
         <v>26.5</v>
       </c>
       <c r="N75">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.5514729444204804</v>
       </c>
-    </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O75">
+        <f t="shared" si="3"/>
+        <v>0.59191215740341341</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>43607.513888888891</v>
       </c>
@@ -4107,11 +4410,15 @@
         <v>26.4</v>
       </c>
       <c r="N76">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.2225758156927373</v>
       </c>
-    </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O76">
+        <f t="shared" si="3"/>
+        <v>1.0370959692821229</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>43607.520833333336</v>
       </c>
@@ -4149,11 +4456,15 @@
         <v>27.6</v>
       </c>
       <c r="N77">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.1698923187963874</v>
       </c>
-    </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O77">
+        <f t="shared" si="3"/>
+        <v>0.86164871979939794</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>43607.527777777781</v>
       </c>
@@ -4191,11 +4502,15 @@
         <v>26.8</v>
       </c>
       <c r="N78">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.2225758156927373</v>
       </c>
-    </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O78">
+        <f t="shared" si="3"/>
+        <v>1.0370959692821229</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>43607.534722222219</v>
       </c>
@@ -4233,11 +4548,15 @@
         <v>26.4</v>
       </c>
       <c r="N79">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.2181552199362242</v>
       </c>
-    </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O79">
+        <f t="shared" si="3"/>
+        <v>0.20302586998937069</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>43607.541666666664</v>
       </c>
@@ -4275,11 +4594,15 @@
         <v>26.2</v>
       </c>
       <c r="N80">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.6709948147273306</v>
       </c>
-    </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O80">
+        <f t="shared" si="3"/>
+        <v>0.27849913578788843</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>43607.548611111109</v>
       </c>
@@ -4317,11 +4640,15 @@
         <v>25.8</v>
       </c>
       <c r="N81">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.7436368079704769</v>
       </c>
-    </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O81">
+        <f t="shared" si="3"/>
+        <v>0.29060613466174617</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>43607.555555555555</v>
       </c>
@@ -4359,11 +4686,15 @@
         <v>25.6</v>
       </c>
       <c r="N82">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.702979787441171</v>
       </c>
-    </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O82">
+        <f t="shared" si="3"/>
+        <v>1.2838299645735285</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>43607.5625</v>
       </c>
@@ -4401,11 +4732,15 @@
         <v>26.3</v>
       </c>
       <c r="N83">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.0449441157225081</v>
       </c>
-    </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O83">
+        <f t="shared" si="3"/>
+        <v>0.50749068595375135</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>43607.569444444445</v>
       </c>
@@ -4443,11 +4778,15 @@
         <v>25.7</v>
       </c>
       <c r="N84">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.8951760636757493</v>
       </c>
-    </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O84">
+        <f t="shared" si="3"/>
+        <v>0.31586267727929157</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>43607.576388888891</v>
       </c>
@@ -4485,11 +4824,15 @@
         <v>25.4</v>
       </c>
       <c r="N85">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.753137374114913</v>
       </c>
-    </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O85">
+        <f t="shared" si="3"/>
+        <v>1.1255228956858188</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>43607.583333333336</v>
       </c>
@@ -4527,11 +4870,15 @@
         <v>25.1</v>
       </c>
       <c r="N86">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.950528105804895</v>
       </c>
-    </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O86">
+        <f t="shared" si="3"/>
+        <v>0.1584213509674825</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>43607.590277777781</v>
       </c>
@@ -4569,11 +4916,15 @@
         <v>25.1</v>
       </c>
       <c r="N87">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.2240940984020772</v>
       </c>
-    </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O87">
+        <f t="shared" si="3"/>
+        <v>0.37068234973367953</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>43607.597222222219</v>
       </c>
@@ -4611,11 +4962,15 @@
         <v>24.8</v>
       </c>
       <c r="N88">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.8565002066501852</v>
       </c>
-    </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O88">
+        <f t="shared" si="3"/>
+        <v>0.30941670110836422</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>43607.604166666664</v>
       </c>
@@ -4653,11 +5008,15 @@
         <v>24.7</v>
       </c>
       <c r="N89">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.7855775863804553</v>
       </c>
-    </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O89">
+        <f t="shared" si="3"/>
+        <v>0.46426293106340921</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>43607.611111111109</v>
       </c>
@@ -4695,11 +5054,15 @@
         <v>24.8</v>
       </c>
       <c r="N90">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.42930012519807281</v>
       </c>
-    </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O90">
+        <f t="shared" si="3"/>
+        <v>7.1550020866345473E-2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>43607.618055555555</v>
       </c>
@@ -4737,11 +5100,15 @@
         <v>23.9</v>
       </c>
       <c r="N91">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.37397947907959983</v>
       </c>
-    </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O91">
+        <f t="shared" si="3"/>
+        <v>6.2329913179933305E-2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>43607.625</v>
       </c>
@@ -4779,11 +5146,15 @@
         <v>24.1</v>
       </c>
       <c r="N92">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.6123083605980516E-2</v>
       </c>
-    </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O92">
+        <f t="shared" si="3"/>
+        <v>6.0205139343300863E-3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>43607.631944444445</v>
       </c>
@@ -4821,11 +5192,15 @@
         <v>24</v>
       </c>
       <c r="N93">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.81052991924273965</v>
       </c>
-    </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O93">
+        <f t="shared" si="3"/>
+        <v>0.13508831987378994</v>
+      </c>
+    </row>
+    <row r="94" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>43607.638888888891</v>
       </c>
@@ -4863,11 +5238,15 @@
         <v>24.5</v>
       </c>
       <c r="N94">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.1893811033215442</v>
       </c>
-    </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O94">
+        <f t="shared" si="3"/>
+        <v>0.19823018388692404</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>43607.645833333336</v>
       </c>
@@ -4905,11 +5284,15 @@
         <v>24.7</v>
       </c>
       <c r="N95">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.62741531654824489</v>
       </c>
-    </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O95">
+        <f t="shared" si="3"/>
+        <v>0.10456921942470748</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>43607.652777777781</v>
       </c>
@@ -4947,11 +5330,15 @@
         <v>24.6</v>
       </c>
       <c r="N96">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.2462934414095432</v>
       </c>
-    </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O96">
+        <f t="shared" si="3"/>
+        <v>0.87438224023492384</v>
+      </c>
+    </row>
+    <row r="97" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>43607.659722222219</v>
       </c>
@@ -4989,11 +5376,15 @@
         <v>25</v>
       </c>
       <c r="N97">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.31178911994912295</v>
       </c>
-    </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O97">
+        <f t="shared" si="3"/>
+        <v>5.1964853324853823E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>43607.666666666664</v>
       </c>
@@ -5031,11 +5422,15 @@
         <v>25.1</v>
       </c>
       <c r="N98">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.2473897126733284</v>
       </c>
-    </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O98">
+        <f t="shared" si="3"/>
+        <v>0.20789828544555475</v>
+      </c>
+    </row>
+    <row r="99" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>43607.673611111109</v>
       </c>
@@ -5073,11 +5468,15 @@
         <v>25.1</v>
       </c>
       <c r="N99">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.30725444162981</v>
       </c>
-    </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O99">
+        <f t="shared" si="3"/>
+        <v>0.217875740271635</v>
+      </c>
+    </row>
+    <row r="100" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>43607.680555555555</v>
       </c>
@@ -5115,11 +5514,15 @@
         <v>24.7</v>
       </c>
       <c r="N100">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.70495093746309279</v>
       </c>
-    </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O100">
+        <f t="shared" si="3"/>
+        <v>0.11749182291051546</v>
+      </c>
+    </row>
+    <row r="101" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>43607.6875</v>
       </c>
@@ -5157,11 +5560,15 @@
         <v>24.2</v>
       </c>
       <c r="N101">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.27801176230025965</v>
       </c>
-    </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O101">
+        <f t="shared" si="3"/>
+        <v>4.6335293716709941E-2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <v>43607.694444444445</v>
       </c>
@@ -5199,11 +5606,15 @@
         <v>24.8</v>
       </c>
       <c r="N102">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.42930012519807281</v>
       </c>
-    </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O102">
+        <f t="shared" si="3"/>
+        <v>7.1550020866345473E-2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
         <v>43607.701388888891</v>
       </c>
@@ -5241,11 +5652,15 @@
         <v>25.1</v>
       </c>
       <c r="N103">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.30024257013788214</v>
       </c>
-    </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O103">
+        <f t="shared" si="3"/>
+        <v>5.0040428356313692E-2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
         <v>43607.708333333336</v>
       </c>
@@ -5283,11 +5698,15 @@
         <v>25.1</v>
       </c>
       <c r="N104">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.0966301998397516</v>
       </c>
-    </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O104">
+        <f t="shared" si="3"/>
+        <v>0.34943836663995859</v>
+      </c>
+    </row>
+    <row r="105" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
         <v>43607.715277777781</v>
       </c>
@@ -5325,11 +5744,15 @@
         <v>26.4</v>
       </c>
       <c r="N105">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.4982776484273894</v>
       </c>
-    </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O105">
+        <f t="shared" si="3"/>
+        <v>0.2497129414045649</v>
+      </c>
+    </row>
+    <row r="106" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
         <v>43607.722222222219</v>
       </c>
@@ -5367,11 +5790,15 @@
         <v>27.2</v>
       </c>
       <c r="N106">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.2181552199362242</v>
       </c>
-    </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O106">
+        <f t="shared" si="3"/>
+        <v>0.20302586998937069</v>
+      </c>
+    </row>
+    <row r="107" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
         <v>43607.729166666664</v>
       </c>
@@ -5409,11 +5836,15 @@
         <v>27.3</v>
       </c>
       <c r="N107">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.59087631112795702</v>
       </c>
-    </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O107">
+        <f t="shared" si="3"/>
+        <v>9.8479385187992832E-2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
         <v>43607.736111111109</v>
       </c>
@@ -5451,11 +5882,15 @@
         <v>26.4</v>
       </c>
       <c r="N108">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.85554934514039349</v>
       </c>
-    </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O108">
+        <f t="shared" si="3"/>
+        <v>0.14259155752339892</v>
+      </c>
+    </row>
+    <row r="109" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
         <v>43607.743055555555</v>
       </c>
@@ -5493,11 +5928,15 @@
         <v>26.4</v>
       </c>
       <c r="N109">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.4982776484273894</v>
       </c>
-    </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O109">
+        <f t="shared" si="3"/>
+        <v>0.2497129414045649</v>
+      </c>
+    </row>
+    <row r="110" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
         <v>43607.75</v>
       </c>
@@ -5535,11 +5974,15 @@
         <v>26.6</v>
       </c>
       <c r="N110">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0788153225120864</v>
       </c>
-    </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O110">
+        <f t="shared" si="3"/>
+        <v>0.1798025537520144</v>
+      </c>
+    </row>
+    <row r="111" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
         <v>43607.756944444445</v>
       </c>
@@ -5577,11 +6020,15 @@
         <v>26.5</v>
       </c>
       <c r="N111">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.27801176230025965</v>
       </c>
-    </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O111">
+        <f t="shared" si="3"/>
+        <v>4.6335293716709941E-2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
         <v>43607.763888888891</v>
       </c>
@@ -5619,11 +6066,15 @@
         <v>27.4</v>
       </c>
       <c r="N112">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.19147749328875519</v>
       </c>
-    </row>
-    <row r="113" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O112">
+        <f t="shared" si="3"/>
+        <v>3.1912915548125864E-2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
         <v>43607.770833333336</v>
       </c>
@@ -5661,11 +6112,15 @@
         <v>27.9</v>
       </c>
       <c r="N113">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.44393411805256006</v>
       </c>
-    </row>
-    <row r="114" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O113">
+        <f t="shared" si="3"/>
+        <v>7.3989019675426676E-2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
         <v>43607.777777777781</v>
       </c>
@@ -5703,11 +6158,15 @@
         <v>29.3</v>
       </c>
       <c r="N114">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.31178911994912295</v>
       </c>
-    </row>
-    <row r="115" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O114">
+        <f t="shared" si="3"/>
+        <v>5.1964853324853823E-2</v>
+      </c>
+    </row>
+    <row r="115" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
         <v>43607.784722222219</v>
       </c>
@@ -5745,11 +6204,15 @@
         <v>30.6</v>
       </c>
       <c r="N115">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.11277570798972246</v>
       </c>
-    </row>
-    <row r="116" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O115">
+        <f t="shared" si="3"/>
+        <v>1.879595133162041E-2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
         <v>43607.791666666664</v>
       </c>
@@ -5787,11 +6250,15 @@
         <v>32.1</v>
       </c>
       <c r="N116">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.3224378516558169E-2</v>
       </c>
-    </row>
-    <row r="117" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O116">
+        <f t="shared" si="3"/>
+        <v>1.0537396419426361E-2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A117" s="1">
         <v>43607.798611111109</v>
       </c>
@@ -5829,11 +6296,15 @@
         <v>33</v>
       </c>
       <c r="N117">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.26732019671637924</v>
       </c>
-    </row>
-    <row r="118" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O117">
+        <f t="shared" si="3"/>
+        <v>4.4553366119396538E-2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A118" s="1">
         <v>43607.805555555555</v>
       </c>
@@ -5871,11 +6342,15 @@
         <v>35.6</v>
       </c>
       <c r="N118">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.12506823762896663</v>
       </c>
-    </row>
-    <row r="119" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O118">
+        <f t="shared" si="3"/>
+        <v>2.0844706271494439E-2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A119" s="1">
         <v>43607.8125</v>
       </c>
@@ -5913,11 +6388,15 @@
         <v>38.299999999999997</v>
       </c>
       <c r="N119">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.25690631831745359</v>
       </c>
-    </row>
-    <row r="120" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O119">
+        <f t="shared" si="3"/>
+        <v>4.2817719719575598E-2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A120" s="1">
         <v>43607.819444444445</v>
       </c>
@@ -5955,11 +6434,15 @@
         <v>38.9</v>
       </c>
       <c r="N120">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.3934686661094398E-2</v>
       </c>
-    </row>
-    <row r="121" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O120">
+        <f t="shared" si="3"/>
+        <v>3.989114443515733E-3</v>
+      </c>
+    </row>
+    <row r="121" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
         <v>43607.826388888891</v>
       </c>
@@ -5997,11 +6480,15 @@
         <v>41.1</v>
       </c>
       <c r="N121">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.15963602941395097</v>
       </c>
-    </row>
-    <row r="122" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O121">
+        <f t="shared" si="3"/>
+        <v>2.6606004902325162E-2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A122" s="1">
         <v>43607.833333333336</v>
       </c>
@@ -6039,11 +6526,15 @@
         <v>42.1</v>
       </c>
       <c r="N122">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.16723649817583572</v>
       </c>
-    </row>
-    <row r="123" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O122">
+        <f t="shared" si="3"/>
+        <v>2.7872749695972619E-2</v>
+      </c>
+    </row>
+    <row r="123" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A123" s="1">
         <v>43607.840277777781</v>
       </c>
@@ -6081,11 +6572,15 @@
         <v>45</v>
       </c>
       <c r="N123">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.6709948147273306</v>
       </c>
-    </row>
-    <row r="124" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O123">
+        <f t="shared" si="3"/>
+        <v>0.27849913578788843</v>
+      </c>
+    </row>
+    <row r="124" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A124" s="1">
         <v>43607.847222222219</v>
       </c>
@@ -6123,11 +6618,15 @@
         <v>46.2</v>
       </c>
       <c r="N124">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.25690631831745359</v>
       </c>
-    </row>
-    <row r="125" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O124">
+        <f t="shared" si="3"/>
+        <v>4.2817719719575598E-2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A125" s="1">
         <v>43607.854166666664</v>
       </c>
@@ -6165,11 +6664,15 @@
         <v>46.6</v>
       </c>
       <c r="N125">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.5889769499352934E-2</v>
       </c>
-    </row>
-    <row r="126" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O125">
+        <f t="shared" si="3"/>
+        <v>1.5981628249892157E-2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A126" s="1">
         <v>43607.861111111109</v>
       </c>
@@ -6207,11 +6710,15 @@
         <v>48.5</v>
       </c>
       <c r="N126">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.11881601322561187</v>
       </c>
-    </row>
-    <row r="127" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O126">
+        <f t="shared" si="3"/>
+        <v>1.9802668870935312E-2</v>
+      </c>
+    </row>
+    <row r="127" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A127" s="1">
         <v>43607.868055555555</v>
       </c>
@@ -6249,11 +6756,15 @@
         <v>48.8</v>
       </c>
       <c r="N127">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.34819719829755691</v>
       </c>
-    </row>
-    <row r="128" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O127">
+        <f t="shared" si="3"/>
+        <v>5.8032866382926152E-2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A128" s="1">
         <v>43607.875</v>
       </c>
@@ -6291,11 +6802,15 @@
         <v>49</v>
       </c>
       <c r="N128">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.1873914831535334E-2</v>
       </c>
-    </row>
-    <row r="129" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O128">
+        <f t="shared" si="3"/>
+        <v>8.6456524719225551E-3</v>
+      </c>
+    </row>
+    <row r="129" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A129" s="1">
         <v>43607.881944444445</v>
       </c>
@@ -6333,11 +6848,15 @@
         <v>49.8</v>
       </c>
       <c r="N129">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.5625087066027866E-2</v>
       </c>
-    </row>
-    <row r="130" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O129">
+        <f t="shared" si="3"/>
+        <v>1.4270847844337978E-2</v>
+      </c>
+    </row>
+    <row r="130" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A130" s="1">
         <v>43607.888888888891</v>
       </c>
@@ -6375,11 +6894,15 @@
         <v>50.6</v>
       </c>
       <c r="N130">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.32362797206031613</v>
       </c>
-    </row>
-    <row r="131" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O130">
+        <f t="shared" si="3"/>
+        <v>5.3937995343386023E-2</v>
+      </c>
+    </row>
+    <row r="131" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A131" s="1">
         <v>43607.895833333336</v>
       </c>
@@ -6417,11 +6940,15 @@
         <v>52</v>
       </c>
       <c r="N131">
-        <f t="shared" ref="N131:N145" si="2">0.5*0.0765*0.000133*0.35*30429.57*(G131*2.24)^3</f>
+        <f t="shared" ref="N131:N145" si="4">0.5*0.0765*0.000133*0.35*30429.57*(G131*2.24)^3</f>
         <v>4.1768780736934257E-3</v>
       </c>
-    </row>
-    <row r="132" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O131">
+        <f t="shared" ref="O131:O145" si="5">N131*1/6</f>
+        <v>6.9614634561557091E-4</v>
+      </c>
+    </row>
+    <row r="132" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A132" s="1">
         <v>43607.902777777781</v>
       </c>
@@ -6459,11 +6986,15 @@
         <v>52.6</v>
       </c>
       <c r="N132">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.6442004372317028E-2</v>
       </c>
-    </row>
-    <row r="133" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O132">
+        <f t="shared" si="5"/>
+        <v>2.7403340620528378E-3</v>
+      </c>
+    </row>
+    <row r="133" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A133" s="1">
         <v>43607.909722222219</v>
       </c>
@@ -6501,11 +7032,15 @@
         <v>52.2</v>
       </c>
       <c r="N133">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.10694366814254919</v>
       </c>
-    </row>
-    <row r="134" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O133">
+        <f t="shared" si="5"/>
+        <v>1.7823944690424864E-2</v>
+      </c>
+    </row>
+    <row r="134" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A134" s="1">
         <v>43607.916666666664</v>
       </c>
@@ -6543,11 +7078,15 @@
         <v>52.9</v>
       </c>
       <c r="N134">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.8973639993640369E-2</v>
       </c>
-    </row>
-    <row r="135" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O134">
+        <f t="shared" si="5"/>
+        <v>6.4956066656067278E-3</v>
+      </c>
+    </row>
+    <row r="135" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A135" s="1">
         <v>43607.923611111109</v>
       </c>
@@ -6585,11 +7124,15 @@
         <v>56.7</v>
       </c>
       <c r="N135">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2.1884307819553965E-2</v>
       </c>
-    </row>
-    <row r="136" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O135">
+        <f t="shared" si="5"/>
+        <v>3.6473846365923275E-3</v>
+      </c>
+    </row>
+    <row r="136" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A136" s="1">
         <v>43607.930555555555</v>
       </c>
@@ -6627,11 +7170,15 @@
         <v>54.8</v>
       </c>
       <c r="N136">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.3367958517818648E-2</v>
       </c>
-    </row>
-    <row r="137" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O136">
+        <f t="shared" si="5"/>
+        <v>2.2279930863031081E-3</v>
+      </c>
+    </row>
+    <row r="137" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A137" s="1">
         <v>43607.9375</v>
       </c>
@@ -6669,11 +7216,15 @@
         <v>54.6</v>
       </c>
       <c r="N137">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.6123083605980516E-2</v>
       </c>
-    </row>
-    <row r="138" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O137">
+        <f t="shared" si="5"/>
+        <v>6.0205139343300863E-3</v>
+      </c>
+    </row>
+    <row r="138" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A138" s="1">
         <v>43607.944444444445</v>
       </c>
@@ -6711,11 +7262,15 @@
         <v>55.4</v>
       </c>
       <c r="N138">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6.3224378516558169E-2</v>
       </c>
-    </row>
-    <row r="139" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O138">
+        <f t="shared" si="5"/>
+        <v>1.0537396419426361E-2</v>
+      </c>
+    </row>
+    <row r="139" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A139" s="1">
         <v>43607.951388888891</v>
       </c>
@@ -6753,11 +7308,15 @@
         <v>56.5</v>
       </c>
       <c r="N139">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.5514729444204775E-3</v>
       </c>
-    </row>
-    <row r="140" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O139">
+        <f t="shared" si="5"/>
+        <v>5.9191215740341289E-4</v>
+      </c>
+    </row>
+    <row r="140" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A140" s="1">
         <v>43607.958333333336</v>
       </c>
@@ -6795,11 +7354,15 @@
         <v>57.4</v>
       </c>
       <c r="N140">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>8.1052991924273959E-4</v>
       </c>
-    </row>
-    <row r="141" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O140">
+        <f t="shared" si="5"/>
+        <v>1.3508831987378992E-4</v>
+      </c>
+    </row>
+    <row r="141" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A141" s="1">
         <v>43607.965277777781</v>
       </c>
@@ -6837,11 +7400,15 @@
         <v>58.4</v>
       </c>
       <c r="N141">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2.4943129595929839E-3</v>
       </c>
-    </row>
-    <row r="142" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O141">
+        <f t="shared" si="5"/>
+        <v>4.1571882659883065E-4</v>
+      </c>
+    </row>
+    <row r="142" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A142" s="1">
         <v>43607.972222222219</v>
       </c>
@@ -6879,11 +7446,15 @@
         <v>58.8</v>
       </c>
       <c r="N142">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>7.6120390612578845E-2</v>
       </c>
-    </row>
-    <row r="143" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O142">
+        <f t="shared" si="5"/>
+        <v>1.2686731768763141E-2</v>
+      </c>
+    </row>
+    <row r="143" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A143" s="1">
         <v>43607.979166666664</v>
       </c>
@@ -6921,11 +7492,15 @@
         <v>60</v>
       </c>
       <c r="N143">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>9.5150488265723556E-3</v>
       </c>
-    </row>
-    <row r="144" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O143">
+        <f t="shared" si="5"/>
+        <v>1.5858414710953927E-3</v>
+      </c>
+    </row>
+    <row r="144" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A144" s="1">
         <v>43607.986111111109</v>
       </c>
@@ -6963,11 +7538,15 @@
         <v>61.4</v>
       </c>
       <c r="N144">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.1986221187419117E-2</v>
       </c>
-    </row>
-    <row r="145" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O144">
+        <f t="shared" si="5"/>
+        <v>1.9977035312365196E-3</v>
+      </c>
+    </row>
+    <row r="145" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A145" s="1">
         <v>43607.993055555555</v>
       </c>
@@ -7005,8 +7584,12 @@
         <v>61.3</v>
       </c>
       <c r="N145">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.8416831171474439E-2</v>
+      </c>
+      <c r="O145">
+        <f t="shared" si="5"/>
+        <v>8.069471861912406E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>